<commit_message>
import and get data
</commit_message>
<xml_diff>
--- a/TemplateFile/Template.xlsx
+++ b/TemplateFile/Template.xlsx
@@ -397,15 +397,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1169,7 +1169,7 @@
       <c r="O20" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uZ8PQOUfsZJfBqkgZSPR2o0jKqmvEBKfRSGH9JmRt1/Cf1FdbF+EBW4QrAiTAKG2rLCyMD3HLSG+p/9kcy9VnA==" saltValue="2PSXtgSGUT5kTiijyGvqug==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="C1:O1"/>
     <mergeCell ref="A1:A4"/>

</xml_diff>

<commit_message>
commit fix bug error function getdata()
</commit_message>
<xml_diff>
--- a/TemplateFile/Template.xlsx
+++ b/TemplateFile/Template.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <x:workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trung-Hieu\Desktop\MTN\TemplateFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="sheet_name" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:calcPr calcId="162913"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205"/>
+  </bookViews>
+  <sheets>
+    <sheet name="sheet_name" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,9 +388,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -407,6 +404,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,31 +710,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -747,8 +750,8 @@
       <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
@@ -791,8 +794,8 @@
       <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
@@ -838,20 +841,20 @@
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="23"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:16" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1169,7 +1172,6 @@
       <c r="O20" s="12"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="C1:O1"/>
     <mergeCell ref="A1:A4"/>

</xml_diff>